<commit_message>
Finzalizacion de subida de excel
</commit_message>
<xml_diff>
--- a/TPI/uploads/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
+++ b/TPI/uploads/Nuevo Hoja de cálculo de Microsoft Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jere\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6507C18-D7D4-4290-8F6F-6273FF849793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAE2D04-001B-437F-8F6E-C0AA1241CE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="3015" windowWidth="15375" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Legajo</t>
   </si>
@@ -39,15 +39,29 @@
     <t>Cupo</t>
   </si>
   <si>
-    <t>F1</t>
+    <t>AM1</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,12 +89,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,58 +383,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
-        <v>44400.666666666664</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>44404.833333333336</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E3" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>